<commit_message>
Completed the driver script
</commit_message>
<xml_diff>
--- a/Abhimanyu_Analysis/FinalSet.xlsx
+++ b/Abhimanyu_Analysis/FinalSet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="464" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -920,12 +920,14 @@
   <dimension ref="A1:F257"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.5748987854251"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="8.5748987854251"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.0242914979757"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.5748987854251"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -965,7 +967,7 @@
         <v>2.8216028260472</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>0.098961832649116</v>
+        <v>0.953011902235774</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -985,7 +987,7 @@
         <v>1.52026619225122</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>0.0235815541663901</v>
+        <v>0.941944168003894</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1005,7 +1007,7 @@
         <v>4.95588486431674</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>0.270133822882557</v>
+        <v>0.902495594449393</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1025,7 +1027,7 @@
         <v>1.57332233136036</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>0.1082104492556</v>
+        <v>0.880182892537037</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1045,7 +1047,7 @@
         <v>0.519594076508675</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>0.0180639338163945</v>
+        <v>0.927362383316519</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1065,7 +1067,7 @@
         <v>2.37652017326988</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>0.0889816866011109</v>
+        <v>0.899347933616979</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1085,7 +1087,7 @@
         <v>0.801974976526803</v>
       </c>
       <c r="F8" s="0" t="n">
-        <v>0.100513629225598</v>
+        <v>0.884831507930872</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1105,7 +1107,7 @@
         <v>3.13643868806776</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>0.117543074375036</v>
+        <v>0.819864398826716</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1125,7 +1127,7 @@
         <v>6.76675733571701</v>
       </c>
       <c r="F10" s="0" t="n">
-        <v>0.209960634225465</v>
+        <v>0.921953367079429</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1145,7 +1147,7 @@
         <v>1.58703473747241</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>0.0192646681450293</v>
+        <v>0.94601366073259</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1165,7 +1167,7 @@
         <v>2.64457384239316</v>
       </c>
       <c r="F12" s="0" t="n">
-        <v>0.111176876491422</v>
+        <v>0.918929405531941</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1185,7 +1187,7 @@
         <v>1.1738277160343</v>
       </c>
       <c r="F13" s="0" t="n">
-        <v>0.0737225595580976</v>
+        <v>0.932116281288232</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1205,7 +1207,7 @@
         <v>0.344628116267002</v>
       </c>
       <c r="F14" s="0" t="n">
-        <v>0.03291995579628</v>
+        <v>0.954780425710092</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1225,7 +1227,7 @@
         <v>3.68991397320531</v>
       </c>
       <c r="F15" s="0" t="n">
-        <v>0.075932449231223</v>
+        <v>0.937437993742434</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1245,7 +1247,7 @@
         <v>3.48398025018142</v>
       </c>
       <c r="F16" s="0" t="n">
-        <v>0.288017725069235</v>
+        <v>0.857096321683657</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1265,7 +1267,7 @@
         <v>0.214061109020702</v>
       </c>
       <c r="F17" s="0" t="n">
-        <v>0.379435149320437</v>
+        <v>0.919584180345172</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1285,7 +1287,7 @@
         <v>1.93662348521513</v>
       </c>
       <c r="F18" s="0" t="n">
-        <v>0.0539362802480361</v>
+        <v>0.940760366053923</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1305,7 +1307,7 @@
         <v>0.684177230993258</v>
       </c>
       <c r="F19" s="0" t="n">
-        <v>0.0297330704422887</v>
+        <v>0.954210309338063</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1325,7 +1327,7 @@
         <v>6.21416219827443</v>
       </c>
       <c r="F20" s="0" t="n">
-        <v>0.276224192457977</v>
+        <v>0.939213930249268</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1345,7 +1347,7 @@
         <v>3.20469349562646</v>
       </c>
       <c r="F21" s="0" t="n">
-        <v>0.153853256728017</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1365,7 +1367,7 @@
         <v>2.92242509966994</v>
       </c>
       <c r="F22" s="0" t="n">
-        <v>0.162484172915323</v>
+        <v>0.929762579851272</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1385,7 +1387,7 @@
         <v>4.66720031712146</v>
       </c>
       <c r="F23" s="0" t="n">
-        <v>0.166553556041023</v>
+        <v>0.93421286637135</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1405,7 +1407,7 @@
         <v>2.63587160946938</v>
       </c>
       <c r="F24" s="0" t="n">
-        <v>0.100585307180202</v>
+        <v>0.873153778380735</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1425,7 +1427,7 @@
         <v>1.99645850234309</v>
       </c>
       <c r="F25" s="0" t="n">
-        <v>0.0288863537399265</v>
+        <v>0.955284624936465</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1445,7 +1447,7 @@
         <v>3.32711303880613</v>
       </c>
       <c r="F26" s="0" t="n">
-        <v>0.16607349833195</v>
+        <v>0.871515748454361</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1465,7 +1467,7 @@
         <v>1.12957280249739</v>
       </c>
       <c r="F27" s="0" t="n">
-        <v>0.0340960614581675</v>
+        <v>0.889130782038333</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1485,7 +1487,7 @@
         <v>0.773997724941688</v>
       </c>
       <c r="F28" s="0" t="n">
-        <v>0.0809815250124841</v>
+        <v>0.950077695217443</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1505,7 +1507,7 @@
         <v>0.681073307866178</v>
       </c>
       <c r="F29" s="0" t="n">
-        <v>0.0377554116719494</v>
+        <v>0.965557565197811</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1525,7 +1527,7 @@
         <v>2.87417721833994</v>
       </c>
       <c r="F30" s="0" t="n">
-        <v>0.141873932281905</v>
+        <v>0.769845988643126</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1545,7 +1547,7 @@
         <v>2.08886679774822</v>
       </c>
       <c r="F31" s="0" t="n">
-        <v>0.0744515985000106</v>
+        <v>0.928876343332407</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1565,7 +1567,7 @@
         <v>3.89561299944838</v>
       </c>
       <c r="F32" s="0" t="n">
-        <v>0.217295814384888</v>
+        <v>0.653482821939298</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1585,7 +1587,7 @@
         <v>2.38325960102395</v>
       </c>
       <c r="F33" s="0" t="n">
-        <v>0.122741001577218</v>
+        <v>0.910242540633648</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1605,7 +1607,7 @@
         <v>3.64653988843373</v>
       </c>
       <c r="F34" s="0" t="n">
-        <v>0.132964698314418</v>
+        <v>0.930037898662122</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1625,7 +1627,7 @@
         <v>2.70990015940265</v>
       </c>
       <c r="F35" s="0" t="n">
-        <v>0.0880151535440902</v>
+        <v>0.922511285509608</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1645,7 +1647,7 @@
         <v>6.29095258519155</v>
       </c>
       <c r="F36" s="0" t="n">
-        <v>0.221126253955096</v>
+        <v>0.677683672411623</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1665,7 +1667,7 @@
         <v>2.54368783109404</v>
       </c>
       <c r="F37" s="0" t="n">
-        <v>0.0820691709980212</v>
+        <v>0.914153164510484</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1685,7 +1687,7 @@
         <v>0.664089073819602</v>
       </c>
       <c r="F38" s="0" t="n">
-        <v>0.0456743662398662</v>
+        <v>0.937722757581849</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1705,7 +1707,7 @@
         <v>2.72353366214824</v>
       </c>
       <c r="F39" s="0" t="n">
-        <v>0.104348611367767</v>
+        <v>0.961505741708853</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1725,7 +1727,7 @@
         <v>2.09767118883765</v>
       </c>
       <c r="F40" s="0" t="n">
-        <v>0.0506274636448839</v>
+        <v>0.94590782784026</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1745,7 +1747,7 @@
         <v>0.567355920891514</v>
       </c>
       <c r="F41" s="0" t="n">
-        <v>0.0250609766775054</v>
+        <v>0.945967254238531</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1765,7 +1767,7 @@
         <v>1.3672020564245</v>
       </c>
       <c r="F42" s="0" t="n">
-        <v>0.0892451893896889</v>
+        <v>0.8658490424806</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1785,7 +1787,7 @@
         <v>1.25779901561296</v>
       </c>
       <c r="F43" s="0" t="n">
-        <v>0.031882832577599</v>
+        <v>0.939305877324434</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1805,7 +1807,7 @@
         <v>6.16220049165887</v>
       </c>
       <c r="F44" s="0" t="n">
-        <v>0.139894568957727</v>
+        <v>0.916655514117082</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1825,7 +1827,7 @@
         <v>2.77604101233084</v>
       </c>
       <c r="F45" s="0" t="n">
-        <v>0.0616227142920696</v>
+        <v>0.925250629377713</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1845,7 +1847,7 @@
         <v>0.68450647468902</v>
       </c>
       <c r="F46" s="0" t="n">
-        <v>0.0743973459050546</v>
+        <v>0.871566613312862</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1865,7 +1867,7 @@
         <v>0.215448658763954</v>
       </c>
       <c r="F47" s="0" t="n">
-        <v>0.0397116720228402</v>
+        <v>0.912975838584247</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1885,7 +1887,7 @@
         <v>1.64330177008939</v>
       </c>
       <c r="F48" s="0" t="n">
-        <v>0.0459010424848065</v>
+        <v>0.793422610048559</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1905,7 +1907,7 @@
         <v>2.63283894082459</v>
       </c>
       <c r="F49" s="0" t="n">
-        <v>0.0814885363360876</v>
+        <v>0.952972400280595</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1925,7 +1927,7 @@
         <v>1.0714420696126</v>
       </c>
       <c r="F50" s="0" t="n">
-        <v>0.0905504826498763</v>
+        <v>0.941179407798046</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1945,7 +1947,7 @@
         <v>0.53978017370733</v>
       </c>
       <c r="F51" s="0" t="n">
-        <v>0.046037925499951</v>
+        <v>0.936493749108696</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1965,7 +1967,7 @@
         <v>1.95783162778239</v>
       </c>
       <c r="F52" s="0" t="n">
-        <v>0.133486755904744</v>
+        <v>0.83241435206761</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1985,7 +1987,7 @@
         <v>3.07308431232177</v>
       </c>
       <c r="F53" s="0" t="n">
-        <v>0.08765615194847</v>
+        <v>0.91722072999044</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2005,7 +2007,7 @@
         <v>1.9091118551902</v>
       </c>
       <c r="F54" s="0" t="n">
-        <v>0.038379902368936</v>
+        <v>0.920467346976684</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2025,7 +2027,7 @@
         <v>4.1585809268189</v>
       </c>
       <c r="F55" s="0" t="n">
-        <v>0.131649324045191</v>
+        <v>0.935846561800761</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2045,7 +2047,7 @@
         <v>11.2058512087493</v>
       </c>
       <c r="F56" s="0" t="n">
-        <v>0.220163277375757</v>
+        <v>0.94443217522028</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2065,7 +2067,7 @@
         <v>0.535027394486811</v>
       </c>
       <c r="F57" s="0" t="n">
-        <v>0.023743936968836</v>
+        <v>0.937128585877076</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2085,7 +2087,7 @@
         <v>0.18514382116375</v>
       </c>
       <c r="F58" s="0" t="n">
-        <v>0.110977293518564</v>
+        <v>0.922562232589777</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2105,7 +2107,7 @@
         <v>1.43151782993708</v>
       </c>
       <c r="F59" s="0" t="n">
-        <v>0.0245171904158226</v>
+        <v>0.94765740499445</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2125,7 +2127,7 @@
         <v>7.90913323872378</v>
       </c>
       <c r="F60" s="0" t="n">
-        <v>0.207778736350802</v>
+        <v>0.891927096278134</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2145,7 +2147,7 @@
         <v>5.4254919842639</v>
       </c>
       <c r="F61" s="0" t="n">
-        <v>0.103307383867549</v>
+        <v>0.902682006766586</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2165,7 +2167,7 @@
         <v>1.23261684726169</v>
       </c>
       <c r="F62" s="0" t="n">
-        <v>0.135385700935694</v>
+        <v>0.904454954964053</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2185,7 +2187,7 @@
         <v>0.49826928327881</v>
       </c>
       <c r="F63" s="0" t="n">
-        <v>0.0911029088110997</v>
+        <v>0.902586198868613</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2205,7 +2207,7 @@
         <v>0.0879780417165703</v>
       </c>
       <c r="F64" s="0" t="n">
-        <v>0.0856729381634213</v>
+        <v>0.909519678536037</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2225,7 +2227,7 @@
         <v>1.2686205212527</v>
       </c>
       <c r="F65" s="0" t="n">
-        <v>0.109098687812855</v>
+        <v>0.894752308953325</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2245,7 +2247,7 @@
         <v>1.01391611753856</v>
       </c>
       <c r="F66" s="0" t="n">
-        <v>0.0409754781836665</v>
+        <v>0.940093531277798</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2265,7 +2267,7 @@
         <v>1.37409540326718</v>
       </c>
       <c r="F67" s="0" t="n">
-        <v>0.0365934632192751</v>
+        <v>0.955406000263873</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2285,7 +2287,7 @@
         <v>1.74044127225883</v>
       </c>
       <c r="F68" s="0" t="n">
-        <v>0.0795732841933852</v>
+        <v>0.835562838163926</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2305,7 +2307,7 @@
         <v>4.03146115195644</v>
       </c>
       <c r="F69" s="0" t="n">
-        <v>0.0215626035082546</v>
+        <v>0.969717310060569</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2325,7 +2327,7 @@
         <v>0.340390821047201</v>
       </c>
       <c r="F70" s="0" t="n">
-        <v>0.220797058827716</v>
+        <v>0.686843657233358</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2345,7 +2347,7 @@
         <v>2.64418746530969</v>
       </c>
       <c r="F71" s="0" t="n">
-        <v>0.157171347017674</v>
+        <v>0.868476144075585</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2365,7 +2367,7 @@
         <v>2.4724226813427</v>
       </c>
       <c r="F72" s="0" t="n">
-        <v>0.0529354687239319</v>
+        <v>0.962325494920862</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2385,7 +2387,7 @@
         <v>1.99625500259312</v>
       </c>
       <c r="F73" s="0" t="n">
-        <v>0.0455185002619231</v>
+        <v>0.959874577840662</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2405,7 +2407,7 @@
         <v>2.03184515854309</v>
       </c>
       <c r="F74" s="0" t="n">
-        <v>0.0824397944914922</v>
+        <v>0.89610090475974</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2425,7 +2427,7 @@
         <v>0.452864060993717</v>
       </c>
       <c r="F75" s="0" t="n">
-        <v>0.0518421498945213</v>
+        <v>0.926849551002492</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2445,7 +2447,7 @@
         <v>2.93700296936744</v>
       </c>
       <c r="F76" s="0" t="n">
-        <v>0.133378460982344</v>
+        <v>0.909745846707761</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2465,7 +2467,7 @@
         <v>10.2314403657118</v>
       </c>
       <c r="F77" s="0" t="n">
-        <v>0.425269968597856</v>
+        <v>0.828228884840483</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2485,7 +2487,7 @@
         <v>2.24182379493119</v>
       </c>
       <c r="F78" s="0" t="n">
-        <v>0.0759931774473453</v>
+        <v>0.912435584363569</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2505,7 +2507,7 @@
         <v>0.285163993508682</v>
       </c>
       <c r="F79" s="0" t="n">
-        <v>0.040269387839942</v>
+        <v>0.929414556990695</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2525,7 +2527,7 @@
         <v>0.308673084711922</v>
       </c>
       <c r="F80" s="0" t="n">
-        <v>0.0320956431943745</v>
+        <v>0.924599760726943</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2545,7 +2547,7 @@
         <v>0.174263225998535</v>
       </c>
       <c r="F81" s="0" t="n">
-        <v>0.224791290015988</v>
+        <v>0.698356611335924</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2565,7 +2567,7 @@
         <v>0.701444624427804</v>
       </c>
       <c r="F82" s="0" t="n">
-        <v>0.0109426822644408</v>
+        <v>0.962341404451749</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2585,7 +2587,7 @@
         <v>0.601759030055533</v>
       </c>
       <c r="F83" s="0" t="n">
-        <v>0.0634820183219308</v>
+        <v>0.889300421380815</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2605,7 +2607,7 @@
         <v>2.76952258728067</v>
       </c>
       <c r="F84" s="0" t="n">
-        <v>0.172021795748094</v>
+        <v>0.844632742819173</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2625,7 +2627,7 @@
         <v>3.94568540576263</v>
       </c>
       <c r="F85" s="0" t="n">
-        <v>0.20640082258876</v>
+        <v>0.929489281810529</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2645,7 +2647,7 @@
         <v>0.251574842125948</v>
       </c>
       <c r="F86" s="0" t="n">
-        <v>0.0289625178042068</v>
+        <v>0.933913592428567</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2665,7 +2667,7 @@
         <v>0.642160629955399</v>
       </c>
       <c r="F87" s="0" t="n">
-        <v>0.0659816554910031</v>
+        <v>0.781920531719138</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2685,7 +2687,7 @@
         <v>0.775193640714369</v>
       </c>
       <c r="F88" s="0" t="n">
-        <v>0.0593415607295857</v>
+        <v>0.928986697179109</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2705,7 +2707,7 @@
         <v>1.92585534251478</v>
       </c>
       <c r="F89" s="0" t="n">
-        <v>0.056455132546348</v>
+        <v>0.926606240904018</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2725,7 +2727,7 @@
         <v>5.84872278825524</v>
       </c>
       <c r="F90" s="0" t="n">
-        <v>0.131735438680551</v>
+        <v>0.878169246602732</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2745,7 +2747,7 @@
         <v>2.58319509417463</v>
       </c>
       <c r="F91" s="0" t="n">
-        <v>0.0823496771693088</v>
+        <v>0.924847158006862</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2765,7 +2767,7 @@
         <v>0.67080869016121</v>
       </c>
       <c r="F92" s="0" t="n">
-        <v>0.0295576069592745</v>
+        <v>0.929716530704568</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2785,7 +2787,7 @@
         <v>1.74054503425339</v>
       </c>
       <c r="F93" s="0" t="n">
-        <v>0.0531955400562805</v>
+        <v>0.915139712036612</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2805,7 +2807,7 @@
         <v>9.42073669900097</v>
       </c>
       <c r="F94" s="0" t="n">
-        <v>0.134975232492805</v>
+        <v>0.92244119804692</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2825,7 +2827,7 @@
         <v>0.595192608047389</v>
       </c>
       <c r="F95" s="0" t="n">
-        <v>0.0382948438003862</v>
+        <v>0.972237190356489</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2845,7 +2847,7 @@
         <v>1.38408850029606</v>
       </c>
       <c r="F96" s="0" t="n">
-        <v>0.066470629259155</v>
+        <v>0.92108361871316</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2865,7 +2867,7 @@
         <v>0.312937481523568</v>
       </c>
       <c r="F97" s="0" t="n">
-        <v>0.104069377961289</v>
+        <v>0.914647051135289</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2885,7 +2887,7 @@
         <v>5.39552110263222</v>
       </c>
       <c r="F98" s="0" t="n">
-        <v>0.0759302185754614</v>
+        <v>0.921482594344839</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2905,7 +2907,7 @@
         <v>1.25735144875228</v>
       </c>
       <c r="F99" s="0" t="n">
-        <v>0.0975005000562377</v>
+        <v>0.927981946130873</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2925,7 +2927,7 @@
         <v>1.32040549153775</v>
       </c>
       <c r="F100" s="0" t="n">
-        <v>0.067483063491068</v>
+        <v>0.979128542929186</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2945,7 +2947,7 @@
         <v>1.13297956350628</v>
       </c>
       <c r="F101" s="0" t="n">
-        <v>0.112985692028844</v>
+        <v>0.901856073755031</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2965,7 +2967,7 @@
         <v>1.32096295925465</v>
       </c>
       <c r="F102" s="0" t="n">
-        <v>0.0752405163327555</v>
+        <v>0.940453229195682</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2985,7 +2987,7 @@
         <v>2.06931954169882</v>
       </c>
       <c r="F103" s="0" t="n">
-        <v>0.0344606869415601</v>
+        <v>0.922847183885589</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3005,7 +3007,7 @@
         <v>0.964400534040207</v>
       </c>
       <c r="F104" s="0" t="n">
-        <v>0.0564056472185743</v>
+        <v>0.906891857559414</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3025,7 +3027,7 @@
         <v>3.39480506775866</v>
       </c>
       <c r="F105" s="0" t="n">
-        <v>0.186557636723864</v>
+        <v>0.963607175231367</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3045,7 +3047,7 @@
         <v>2.43372541843507</v>
       </c>
       <c r="F106" s="0" t="n">
-        <v>0.107600744495883</v>
+        <v>0.966697805800107</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3065,7 +3067,7 @@
         <v>0.775675071696862</v>
       </c>
       <c r="F107" s="0" t="n">
-        <v>0.0374963180964996</v>
+        <v>0.950463963160915</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3085,7 +3087,7 @@
         <v>1.77447228783968</v>
       </c>
       <c r="F108" s="0" t="n">
-        <v>0.0390981581078652</v>
+        <v>0.94429737556187</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3105,7 +3107,7 @@
         <v>0.631039132032533</v>
       </c>
       <c r="F109" s="0" t="n">
-        <v>0.117976084430261</v>
+        <v>0.878735477249398</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3125,7 +3127,7 @@
         <v>5.70315336996791</v>
       </c>
       <c r="F110" s="0" t="n">
-        <v>0.196565159199476</v>
+        <v>0.882307832446237</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3145,7 +3147,7 @@
         <v>2.83086017110134</v>
       </c>
       <c r="F111" s="0" t="n">
-        <v>0.0720068058457491</v>
+        <v>0.943704037686971</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3165,7 +3167,7 @@
         <v>0.451004935742556</v>
       </c>
       <c r="F112" s="0" t="n">
-        <v>0.104697895229425</v>
+        <v>0.919603168403494</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3185,7 +3187,7 @@
         <v>0.970331849531614</v>
       </c>
       <c r="F113" s="0" t="n">
-        <v>0.0564849952402562</v>
+        <v>0.912798779419651</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3205,7 +3207,7 @@
         <v>0.482801881228126</v>
       </c>
       <c r="F114" s="0" t="n">
-        <v>0.105500912800308</v>
+        <v>0.849771524534867</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3225,7 +3227,7 @@
         <v>0.410981974981373</v>
       </c>
       <c r="F115" s="0" t="n">
-        <v>0.0450366870237325</v>
+        <v>0.942739144182582</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3245,7 +3247,7 @@
         <v>9.56816509894989</v>
       </c>
       <c r="F116" s="0" t="n">
-        <v>0.265768940944848</v>
+        <v>0.893479300878232</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3265,7 +3267,7 @@
         <v>0.673943304742427</v>
       </c>
       <c r="F117" s="0" t="n">
-        <v>0.124275095595988</v>
+        <v>0.585751945353448</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3285,7 +3287,7 @@
         <v>0.926516524421184</v>
       </c>
       <c r="F118" s="0" t="n">
-        <v>0.0411908186227152</v>
+        <v>0.924748094741008</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3305,7 +3307,7 @@
         <v>3.34133250991551</v>
       </c>
       <c r="F119" s="0" t="n">
-        <v>0.0531297626800139</v>
+        <v>0.95531271332346</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3325,7 +3327,7 @@
         <v>5.35590174952354</v>
       </c>
       <c r="F120" s="0" t="n">
-        <v>0.292118143963995</v>
+        <v>0.916240488909133</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3345,7 +3347,7 @@
         <v>3.66797857563465</v>
       </c>
       <c r="F121" s="0" t="n">
-        <v>0.1833969859312</v>
+        <v>0.741289797027962</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3365,7 +3367,7 @@
         <v>2.58388747537616</v>
       </c>
       <c r="F122" s="0" t="n">
-        <v>0.115413446004239</v>
+        <v>0.903009473583354</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3385,7 +3387,7 @@
         <v>0.950399742786182</v>
       </c>
       <c r="F123" s="0" t="n">
-        <v>0.0791606385900315</v>
+        <v>0.939555438598352</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3405,7 +3407,7 @@
         <v>1.9368087215129</v>
       </c>
       <c r="F124" s="0" t="n">
-        <v>0.094561174861939</v>
+        <v>0.893620873277765</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3425,7 +3427,7 @@
         <v>5.69181386509258</v>
       </c>
       <c r="F125" s="0" t="n">
-        <v>0.159438671562545</v>
+        <v>0.900888976141679</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3445,7 +3447,7 @@
         <v>1.29283520428058</v>
       </c>
       <c r="F126" s="0" t="n">
-        <v>0.142481647994541</v>
+        <v>0.823387440129976</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3465,7 +3467,7 @@
         <v>2.07354792827148</v>
       </c>
       <c r="F127" s="0" t="n">
-        <v>0.0607371196838493</v>
+        <v>0.90711004371899</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3485,7 +3487,7 @@
         <v>1.9649388302761</v>
       </c>
       <c r="F128" s="0" t="n">
-        <v>0.105881501223702</v>
+        <v>0.939597490484769</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3505,7 +3507,7 @@
         <v>0.87423053661346</v>
       </c>
       <c r="F129" s="0" t="n">
-        <v>0.196307768458532</v>
+        <v>0.926900244105684</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3525,7 +3527,7 @@
         <v>2.11195456259752</v>
       </c>
       <c r="F130" s="0" t="n">
-        <v>0.101340411972372</v>
+        <v>0.788960533488682</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3545,7 +3547,7 @@
         <v>1.97948376915761</v>
       </c>
       <c r="F131" s="0" t="n">
-        <v>0.0609608551793581</v>
+        <v>0.935640147223943</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3565,7 +3567,7 @@
         <v>1.3142802222251</v>
       </c>
       <c r="F132" s="0" t="n">
-        <v>0.0374975452215832</v>
+        <v>0.941951124533143</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3585,7 +3587,7 @@
         <v>0.56255287204736</v>
       </c>
       <c r="F133" s="0" t="n">
-        <v>0.0137572423394384</v>
+        <v>0.961926566737773</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3605,7 +3607,7 @@
         <v>0.0350134038126076</v>
       </c>
       <c r="F134" s="0" t="n">
-        <v>0.0193016067489122</v>
+        <v>0.951800177919399</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3625,7 +3627,7 @@
         <v>0.907351626831419</v>
       </c>
       <c r="F135" s="0" t="n">
-        <v>0.0439371009510519</v>
+        <v>0.946677604810052</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3645,7 +3647,7 @@
         <v>2.33572771471804</v>
       </c>
       <c r="F136" s="0" t="n">
-        <v>0.0614869166346844</v>
+        <v>0.930378502536085</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3665,7 +3667,7 @@
         <v>9.7510525824582</v>
       </c>
       <c r="F137" s="0" t="n">
-        <v>0.205551194634061</v>
+        <v>0.913284751281351</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3685,7 +3687,7 @@
         <v>0.931746184545195</v>
       </c>
       <c r="F138" s="0" t="n">
-        <v>0.0770447553858097</v>
+        <v>0.932042813655557</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3705,7 +3707,7 @@
         <v>2.04436157076241</v>
       </c>
       <c r="F139" s="0" t="n">
-        <v>0.0352386281894526</v>
+        <v>0.959824389128633</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3725,7 +3727,7 @@
         <v>0.622484695458597</v>
       </c>
       <c r="F140" s="0" t="n">
-        <v>0.126546452860583</v>
+        <v>0.879862357928242</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3745,7 +3747,7 @@
         <v>8.76437559726088</v>
       </c>
       <c r="F141" s="0" t="n">
-        <v>0.227196808009579</v>
+        <v>0.897639090499969</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3765,7 +3767,7 @@
         <v>6.85520222193374</v>
       </c>
       <c r="F142" s="0" t="n">
-        <v>0.127688980627332</v>
+        <v>0.891077625044595</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3785,7 +3787,7 @@
         <v>15.5237198933853</v>
       </c>
       <c r="F143" s="0" t="n">
-        <v>0.420479010514755</v>
+        <v>0.923923890133092</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3805,7 +3807,7 @@
         <v>9.16083805189704</v>
       </c>
       <c r="F144" s="0" t="n">
-        <v>0.355435742185243</v>
+        <v>0.933529508611513</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3825,7 +3827,7 @@
         <v>0.856663177697821</v>
       </c>
       <c r="F145" s="0" t="n">
-        <v>0.0648932944623116</v>
+        <v>0.882625767211215</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3845,7 +3847,7 @@
         <v>6.05921457547683</v>
       </c>
       <c r="F146" s="0" t="n">
-        <v>0.165223655195053</v>
+        <v>0.92636844779619</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3865,7 +3867,7 @@
         <v>0.626522244758272</v>
       </c>
       <c r="F147" s="0" t="n">
-        <v>0.106603227830119</v>
+        <v>0.758092639175027</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3885,7 +3887,7 @@
         <v>4.92964904853342</v>
       </c>
       <c r="F148" s="0" t="n">
-        <v>0.107951697165029</v>
+        <v>0.896753328690969</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3905,7 +3907,7 @@
         <v>3.72393622301121</v>
       </c>
       <c r="F149" s="0" t="n">
-        <v>0.158090355941045</v>
+        <v>0.863628818840788</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3925,7 +3927,7 @@
         <v>1.85360442156911</v>
       </c>
       <c r="F150" s="0" t="n">
-        <v>0.170894059059417</v>
+        <v>0.705740126698181</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3945,7 +3947,7 @@
         <v>1.17546322594694</v>
       </c>
       <c r="F151" s="0" t="n">
-        <v>0.0525285151732413</v>
+        <v>0.916773409382084</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3965,7 +3967,7 @@
         <v>2.39126198787002</v>
       </c>
       <c r="F152" s="0" t="n">
-        <v>0.170630352905329</v>
+        <v>0.759662052134491</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3985,7 +3987,7 @@
         <v>1.61695713684776</v>
       </c>
       <c r="F153" s="0" t="n">
-        <v>0.10692334650288</v>
+        <v>0.792419414365264</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4005,7 +4007,7 @@
         <v>2.11906898322339</v>
       </c>
       <c r="F154" s="0" t="n">
-        <v>0.112920519740724</v>
+        <v>0.932478145224232</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4025,7 +4027,7 @@
         <v>2.01719554070143</v>
       </c>
       <c r="F155" s="0" t="n">
-        <v>0.0731684757816751</v>
+        <v>0.950188485663913</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4045,7 +4047,7 @@
         <v>9.94251566413261</v>
       </c>
       <c r="F156" s="0" t="n">
-        <v>0.190705456859218</v>
+        <v>0.915985571628578</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4065,7 +4067,7 @@
         <v>0.835814795675844</v>
       </c>
       <c r="F157" s="0" t="n">
-        <v>0.02780951977889</v>
+        <v>0.952527581182259</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4085,7 +4087,7 @@
         <v>0.67175589522808</v>
       </c>
       <c r="F158" s="0" t="n">
-        <v>0.0654646257188563</v>
+        <v>0.941484952918473</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4105,7 +4107,7 @@
         <v>0.661615970385238</v>
       </c>
       <c r="F159" s="0" t="n">
-        <v>0.0376833713418001</v>
+        <v>0.942469971941234</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4125,7 +4127,7 @@
         <v>4.07488494955551</v>
       </c>
       <c r="F160" s="0" t="n">
-        <v>0.105204894664495</v>
+        <v>0.475598484582173</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4145,7 +4147,7 @@
         <v>1.90317825487256</v>
       </c>
       <c r="F161" s="0" t="n">
-        <v>0.142459512927625</v>
+        <v>0.91789850556803</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4165,7 +4167,7 @@
         <v>1.58716688602999</v>
       </c>
       <c r="F162" s="0" t="n">
-        <v>0.0542274470490278</v>
+        <v>0.862383425122454</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4185,7 +4187,7 @@
         <v>0.678386606565316</v>
       </c>
       <c r="F163" s="0" t="n">
-        <v>0.0387632109761012</v>
+        <v>0.89566352450426</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4205,7 +4207,7 @@
         <v>2.04018724637152</v>
       </c>
       <c r="F164" s="0" t="n">
-        <v>0.0574091601846821</v>
+        <v>0.891569198205196</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4225,7 +4227,7 @@
         <v>0.780049872855154</v>
       </c>
       <c r="F165" s="0" t="n">
-        <v>0.063512941999621</v>
+        <v>0.914438101259791</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4245,7 +4247,7 @@
         <v>1.81099010117409</v>
       </c>
       <c r="F166" s="0" t="n">
-        <v>0.138540942164097</v>
+        <v>0.78681764550198</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4265,7 +4267,7 @@
         <v>0.680735445699897</v>
       </c>
       <c r="F167" s="0" t="n">
-        <v>0.0301183103149954</v>
+        <v>0.960881938908227</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4285,7 +4287,7 @@
         <v>2.60772972676737</v>
       </c>
       <c r="F168" s="0" t="n">
-        <v>0.27669977087593</v>
+        <v>0</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4305,7 +4307,7 @@
         <v>1.4440095869474</v>
       </c>
       <c r="F169" s="0" t="n">
-        <v>0.0675968227386518</v>
+        <v>0.920941752383898</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4325,7 +4327,7 @@
         <v>2.88713464569737</v>
       </c>
       <c r="F170" s="0" t="n">
-        <v>0.159609031978931</v>
+        <v>0.829155047512997</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4345,7 +4347,7 @@
         <v>8.02680967994319</v>
       </c>
       <c r="F171" s="0" t="n">
-        <v>0.314790882190524</v>
+        <v>0.908911317242685</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4365,7 +4367,7 @@
         <v>0.509864395169458</v>
       </c>
       <c r="F172" s="0" t="n">
-        <v>0.0245987796716119</v>
+        <v>0.881528767895758</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4385,7 +4387,7 @@
         <v>2.19886921008749</v>
       </c>
       <c r="F173" s="0" t="n">
-        <v>0.150611040094743</v>
+        <v>0.853310444933679</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4405,7 +4407,7 @@
         <v>6.03333307340335</v>
       </c>
       <c r="F174" s="0" t="n">
-        <v>0.216449550964607</v>
+        <v>0.945891063360864</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4425,7 +4427,7 @@
         <v>4.21049049580302</v>
       </c>
       <c r="F175" s="0" t="n">
-        <v>0.143501524596279</v>
+        <v>0.928546052852574</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4445,7 +4447,7 @@
         <v>4.34477066849183</v>
       </c>
       <c r="F176" s="0" t="n">
-        <v>0.215389423287265</v>
+        <v>0.940083433743697</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4465,7 +4467,7 @@
         <v>0.875831997939559</v>
       </c>
       <c r="F177" s="0" t="n">
-        <v>0.0943444489999049</v>
+        <v>0.91398221234042</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4485,7 +4487,7 @@
         <v>0.832459657254328</v>
       </c>
       <c r="F178" s="0" t="n">
-        <v>0.0303476691393524</v>
+        <v>0.926503178123782</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4505,7 +4507,7 @@
         <v>5.31102462135896</v>
       </c>
       <c r="F179" s="0" t="n">
-        <v>0.0734535333276519</v>
+        <v>0.907762615837652</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4525,7 +4527,7 @@
         <v>0.647486170160962</v>
       </c>
       <c r="F180" s="0" t="n">
-        <v>0.089998503651936</v>
+        <v>0.875386127710825</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4545,7 +4547,7 @@
         <v>2.34524221143034</v>
       </c>
       <c r="F181" s="0" t="n">
-        <v>0.0539572633861179</v>
+        <v>0.951718299661425</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4565,7 +4567,7 @@
         <v>2.05167318164928</v>
       </c>
       <c r="F182" s="0" t="n">
-        <v>0.0361442603375387</v>
+        <v>0.95878635443187</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4585,7 +4587,7 @@
         <v>2.29189163931261</v>
       </c>
       <c r="F183" s="0" t="n">
-        <v>0.326070496443186</v>
+        <v>0.957234311089742</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4605,7 +4607,7 @@
         <v>0.529706528346418</v>
       </c>
       <c r="F184" s="0" t="n">
-        <v>0.0247083272093277</v>
+        <v>0.950892105917186</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4625,7 +4627,7 @@
         <v>1.19393973739442</v>
       </c>
       <c r="F185" s="0" t="n">
-        <v>0.0886800031683712</v>
+        <v>0.902835738115497</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4645,7 +4647,7 @@
         <v>1.90515782604522</v>
       </c>
       <c r="F186" s="0" t="n">
-        <v>0.097280698092291</v>
+        <v>0.901211449252512</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4665,7 +4667,7 @@
         <v>0.779691466387337</v>
       </c>
       <c r="F187" s="0" t="n">
-        <v>0.024926951650012</v>
+        <v>0.957914432233599</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4685,7 +4687,7 @@
         <v>1.42867944091334</v>
       </c>
       <c r="F188" s="0" t="n">
-        <v>0.114259178020946</v>
+        <v>0.856769788200106</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4705,7 +4707,7 @@
         <v>7.41511963354939</v>
       </c>
       <c r="F189" s="0" t="n">
-        <v>0.206927474788705</v>
+        <v>0.876474539361099</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4725,7 +4727,7 @@
         <v>1.82705557418848</v>
       </c>
       <c r="F190" s="0" t="n">
-        <v>0.0560052279481869</v>
+        <v>0.91495503810731</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4745,7 +4747,7 @@
         <v>2.91402634920293</v>
       </c>
       <c r="F191" s="0" t="n">
-        <v>0.106335664594541</v>
+        <v>0.915931460019673</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4765,7 +4767,7 @@
         <v>2.48310091511982</v>
       </c>
       <c r="F192" s="0" t="n">
-        <v>0.228456600484859</v>
+        <v>0.872408753191546</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4785,7 +4787,7 @@
         <v>4.39853160174152</v>
       </c>
       <c r="F193" s="0" t="n">
-        <v>0.083780688517468</v>
+        <v>0.952502130991747</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4805,7 +4807,7 @@
         <v>2.24733680800803</v>
       </c>
       <c r="F194" s="0" t="n">
-        <v>0.137375104637039</v>
+        <v>0.747838276465336</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4825,7 +4827,7 @@
         <v>6.99621135865858</v>
       </c>
       <c r="F195" s="0" t="n">
-        <v>0.229188572685541</v>
+        <v>0.797802722420992</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4845,7 +4847,7 @@
         <v>12.3598396439452</v>
       </c>
       <c r="F196" s="0" t="n">
-        <v>0.272728920681833</v>
+        <v>0.940228132159921</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4865,7 +4867,7 @@
         <v>2.5396458747906</v>
       </c>
       <c r="F197" s="0" t="n">
-        <v>0.0816421117605867</v>
+        <v>0.883375942539665</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4885,7 +4887,7 @@
         <v>7.75923413480403</v>
       </c>
       <c r="F198" s="0" t="n">
-        <v>0.180977507219229</v>
+        <v>0.915758503488228</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4905,7 +4907,7 @@
         <v>2.37000440162281</v>
       </c>
       <c r="F199" s="0" t="n">
-        <v>0.0790356936137312</v>
+        <v>0.895845323173849</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4925,7 +4927,7 @@
         <v>1.85083289604356</v>
       </c>
       <c r="F200" s="0" t="n">
-        <v>0.070538877465834</v>
+        <v>0.957759359209608</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4945,7 +4947,7 @@
         <v>0.576143651486382</v>
       </c>
       <c r="F201" s="0" t="n">
-        <v>0.0456008678534293</v>
+        <v>0.872665536360192</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4965,7 +4967,7 @@
         <v>0.753438452233968</v>
       </c>
       <c r="F202" s="0" t="n">
-        <v>0.0936219557680158</v>
+        <v>0.833746658578399</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4985,7 +4987,7 @@
         <v>0.305615344460468</v>
       </c>
       <c r="F203" s="0" t="n">
-        <v>0.0209601784856533</v>
+        <v>0.955955744163097</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5005,7 +5007,7 @@
         <v>0.460206343279802</v>
       </c>
       <c r="F204" s="0" t="n">
-        <v>0.0752166185063666</v>
+        <v>0.867999149337303</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5025,7 +5027,7 @@
         <v>2.19469113704187</v>
       </c>
       <c r="F205" s="0" t="n">
-        <v>0.122893340495171</v>
+        <v>0.921954660538793</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5045,7 +5047,7 @@
         <v>2.0084173683281</v>
       </c>
       <c r="F206" s="0" t="n">
-        <v>0.221882731348694</v>
+        <v>0.886347431180758</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5065,7 +5067,7 @@
         <v>2.14575647239581</v>
       </c>
       <c r="F207" s="0" t="n">
-        <v>0.0580794417746292</v>
+        <v>0.926801105542472</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5085,7 +5087,7 @@
         <v>0.515584715321255</v>
       </c>
       <c r="F208" s="0" t="n">
-        <v>0.0594388691396534</v>
+        <v>0.933303422924797</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5105,7 +5107,7 @@
         <v>1.25307013400771</v>
       </c>
       <c r="F209" s="0" t="n">
-        <v>0.0603080948386124</v>
+        <v>0.926790971751312</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5125,7 +5127,7 @@
         <v>1.86678714553572</v>
       </c>
       <c r="F210" s="0" t="n">
-        <v>0.0589854210683545</v>
+        <v>0.92624320331236</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5145,7 +5147,7 @@
         <v>2.89383525659826</v>
       </c>
       <c r="F211" s="0" t="n">
-        <v>0.0838452428851003</v>
+        <v>0.911005009144619</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5165,7 +5167,7 @@
         <v>1.34665293826959</v>
       </c>
       <c r="F212" s="0" t="n">
-        <v>0.0481661957449417</v>
+        <v>0.943218925087789</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5185,7 +5187,7 @@
         <v>4.97873781895735</v>
       </c>
       <c r="F213" s="0" t="n">
-        <v>0.096925695788165</v>
+        <v>0.879436892625497</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5205,7 +5207,7 @@
         <v>2.1399125641163</v>
       </c>
       <c r="F214" s="0" t="n">
-        <v>0.0775507588217083</v>
+        <v>0.949302442696363</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5225,7 +5227,7 @@
         <v>6.89731671339968</v>
       </c>
       <c r="F215" s="0" t="n">
-        <v>0.195548908243425</v>
+        <v>0.901900572672756</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5245,7 +5247,7 @@
         <v>0.494467790456811</v>
       </c>
       <c r="F216" s="0" t="n">
-        <v>0.101699227830853</v>
+        <v>0.844254617669969</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5265,7 +5267,7 @@
         <v>0.988800289110464</v>
       </c>
       <c r="F217" s="0" t="n">
-        <v>0.0224523392466499</v>
+        <v>0.934243775401227</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5285,7 +5287,7 @@
         <v>7.50496978935372</v>
       </c>
       <c r="F218" s="0" t="n">
-        <v>0.356886570734992</v>
+        <v>0.899476367994142</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5305,7 +5307,7 @@
         <v>3.45650893484577</v>
       </c>
       <c r="F219" s="0" t="n">
-        <v>0.248059700330133</v>
+        <v>0.885230517578073</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5325,7 +5327,7 @@
         <v>12.4048109004884</v>
       </c>
       <c r="F220" s="0" t="n">
-        <v>0.256744525748929</v>
+        <v>0.891496234589472</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5345,7 +5347,7 @@
         <v>7.30784321441215</v>
       </c>
       <c r="F221" s="0" t="n">
-        <v>0.183791707516714</v>
+        <v>0.901484110132997</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5365,7 +5367,7 @@
         <v>0.275862068965517</v>
       </c>
       <c r="F222" s="0" t="n">
-        <v>0.0250134455382289</v>
+        <v>0.965898304792848</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5385,7 +5387,7 @@
         <v>1.64902377817521</v>
       </c>
       <c r="F223" s="0" t="n">
-        <v>0.0775713078340129</v>
+        <v>0.919165456008833</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5405,7 +5407,7 @@
         <v>0.0131324870373681</v>
       </c>
       <c r="F224" s="0" t="n">
-        <v>0.122517208751099</v>
+        <v>0.725132632715764</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5425,7 +5427,7 @@
         <v>2.05753561369404</v>
       </c>
       <c r="F225" s="0" t="n">
-        <v>0.160374162340862</v>
+        <v>0.867457175673106</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5445,7 +5447,7 @@
         <v>0.282724636994897</v>
       </c>
       <c r="F226" s="0" t="n">
-        <v>0.0620284271821874</v>
+        <v>0.922173429657428</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5465,7 +5467,7 @@
         <v>5.8228124593877</v>
       </c>
       <c r="F227" s="0" t="n">
-        <v>0.238187839532371</v>
+        <v>0.935857153159437</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5485,7 +5487,7 @@
         <v>2.30032820855909</v>
       </c>
       <c r="F228" s="0" t="n">
-        <v>0.121217854790511</v>
+        <v>0.785733590132365</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5505,7 +5507,7 @@
         <v>4.10008659343057</v>
       </c>
       <c r="F229" s="0" t="n">
-        <v>0.235008893736668</v>
+        <v>0.808037043509774</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5525,7 +5527,7 @@
         <v>1.91825341844681</v>
       </c>
       <c r="F230" s="0" t="n">
-        <v>0.113166931908109</v>
+        <v>0.854908687831886</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5545,7 +5547,7 @@
         <v>3.66325284741045</v>
       </c>
       <c r="F231" s="0" t="n">
-        <v>0.134245840402619</v>
+        <v>0.88353625225305</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5565,7 +5567,7 @@
         <v>1.13880719689711</v>
       </c>
       <c r="F232" s="0" t="n">
-        <v>0.0917305911159354</v>
+        <v>0.939276226840062</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5585,7 +5587,7 @@
         <v>8.34939673464152</v>
       </c>
       <c r="F233" s="0" t="n">
-        <v>0.247610615942559</v>
+        <v>0.898019739899422</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5605,7 +5607,7 @@
         <v>0.317620578374094</v>
       </c>
       <c r="F234" s="0" t="n">
-        <v>0.0518165530389179</v>
+        <v>0.919111395646817</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5625,7 +5627,7 @@
         <v>0.192036011729106</v>
       </c>
       <c r="F235" s="0" t="n">
-        <v>0.00764656579858075</v>
+        <v>0.999429081414308</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5645,7 +5647,7 @@
         <v>0.680985167415716</v>
       </c>
       <c r="F236" s="0" t="n">
-        <v>0.0260032974132823</v>
+        <v>0.925258412981017</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5665,7 +5667,7 @@
         <v>1.24157029618813</v>
       </c>
       <c r="F237" s="0" t="n">
-        <v>0.064642124332336</v>
+        <v>0.96556050994648</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5685,7 +5687,7 @@
         <v>2.73672885301636</v>
       </c>
       <c r="F238" s="0" t="n">
-        <v>0.0744049997087639</v>
+        <v>0.935135231410187</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5705,7 +5707,7 @@
         <v>0.0860926565243074</v>
       </c>
       <c r="F239" s="0" t="n">
-        <v>0.0619245913331639</v>
+        <v>0.941095630677128</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5725,7 +5727,7 @@
         <v>1.45736330492718</v>
       </c>
       <c r="F240" s="0" t="n">
-        <v>0.0822270560429568</v>
+        <v>0.935452752137234</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5745,7 +5747,7 @@
         <v>3.00865916399996</v>
       </c>
       <c r="F241" s="0" t="n">
-        <v>0.099894035627082</v>
+        <v>0.93306925220232</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5765,7 +5767,7 @@
         <v>5.56856818991173</v>
       </c>
       <c r="F242" s="0" t="n">
-        <v>0.264361541677729</v>
+        <v>0.935720584466816</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5785,7 +5787,7 @@
         <v>0.362644024526177</v>
       </c>
       <c r="F243" s="0" t="n">
-        <v>0.016910200087295</v>
+        <v>0.944848384847736</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5805,7 +5807,7 @@
         <v>0.737809286354542</v>
       </c>
       <c r="F244" s="0" t="n">
-        <v>0.042237580976509</v>
+        <v>0.778502391586166</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5825,7 +5827,7 @@
         <v>1.24011559987628</v>
       </c>
       <c r="F245" s="0" t="n">
-        <v>0.0491702743295292</v>
+        <v>0.954498196080965</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5845,7 +5847,7 @@
         <v>0.814163968805558</v>
       </c>
       <c r="F246" s="0" t="n">
-        <v>0.0983911001882876</v>
+        <v>0.875386530449886</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5865,7 +5867,7 @@
         <v>0.433321494977091</v>
       </c>
       <c r="F247" s="0" t="n">
-        <v>0.0434938610575933</v>
+        <v>0.93035068697962</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5885,7 +5887,7 @@
         <v>1.52699718961072</v>
       </c>
       <c r="F248" s="0" t="n">
-        <v>0.261993198188152</v>
+        <v>0</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5905,7 +5907,7 @@
         <v>2.27944656981563</v>
       </c>
       <c r="F249" s="0" t="n">
-        <v>0.115774955824681</v>
+        <v>0.902124123317633</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5925,7 +5927,7 @@
         <v>2.57348334495844</v>
       </c>
       <c r="F250" s="0" t="n">
-        <v>0.0665641191740012</v>
+        <v>0.951770437883395</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5945,7 +5947,7 @@
         <v>1.81146389564798</v>
       </c>
       <c r="F251" s="0" t="n">
-        <v>0.0837425328622471</v>
+        <v>0.795722517677672</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5965,7 +5967,7 @@
         <v>0.769907039075179</v>
       </c>
       <c r="F252" s="0" t="n">
-        <v>0.112591018541358</v>
+        <v>0.9155965656412</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5985,7 +5987,7 @@
         <v>1.90454337452145</v>
       </c>
       <c r="F253" s="0" t="n">
-        <v>0.0844365917209674</v>
+        <v>0.744982878935189</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6005,7 +6007,7 @@
         <v>0.835382132653318</v>
       </c>
       <c r="F254" s="0" t="n">
-        <v>0.0757156131838965</v>
+        <v>0.886510893153397</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6025,7 +6027,7 @@
         <v>3.19969661052195</v>
       </c>
       <c r="F255" s="0" t="n">
-        <v>0.122077692125162</v>
+        <v>0.884390393957905</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6045,7 +6047,7 @@
         <v>3.1725866838001</v>
       </c>
       <c r="F256" s="0" t="n">
-        <v>0.0646349620180981</v>
+        <v>0.944353000150135</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6065,7 +6067,7 @@
         <v>1.51673575422442</v>
       </c>
       <c r="F257" s="0" t="n">
-        <v>0.0702605232395841</v>
+        <v>0.963349338286231</v>
       </c>
     </row>
   </sheetData>

</xml_diff>